<commit_message>
Update to Training 0003 and 0004.
</commit_message>
<xml_diff>
--- a/taurus/Training_0003-Linear_Autoencoder_SweepEachBit/Training_0003_again.xlsx
+++ b/taurus/Training_0003-Linear_Autoencoder_SweepEachBit/Training_0003_again.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\AGH\Projects\ANN\CNN_autoencoder\results\taurus\Training_0003-Linear_Autoencoder_SweepEachBit\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0EC78052-B28A-4CAD-98E3-0673D786F04E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B528EF1-27EB-439F-A8F8-5044E25AE5BB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{BD5D6309-99CE-4C87-926D-29892797E216}"/>
   </bookViews>
@@ -285,10 +285,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>v_batch_size!$C$10:$C$15</c:f>
+              <c:f>v_batch_size!$C$10:$C$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -306,16 +306,22 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>v_batch_size!$D$10:$D$15</c:f>
+              <c:f>v_batch_size!$D$10:$D$18</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>6.5000000000000002E-2</c:v>
                 </c:pt>
@@ -333,6 +339,12 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6.4899999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.7900000000000002E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.49E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -384,10 +396,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>v_batch_size!$C$10:$C$15</c:f>
+              <c:f>v_batch_size!$C$10:$C$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -405,16 +417,22 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>256</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>v_batch_size!$E$10:$E$15</c:f>
+              <c:f>v_batch_size!$E$10:$E$18</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>6.2600000000000003E-2</c:v>
                 </c:pt>
@@ -432,6 +450,12 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>6.2300000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.2199999999999998E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>6.2199999999999998E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -876,10 +900,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>v_n_bottleneck!$C$10:$C$14</c:f>
+              <c:f>v_n_bottleneck!$C$10:$C$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -894,16 +918,25 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>512</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>v_n_bottleneck!$D$10:$D$14</c:f>
+              <c:f>v_n_bottleneck!$D$10:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>6.5100000000000005E-2</c:v>
                 </c:pt>
@@ -917,6 +950,15 @@
                   <c:v>6.5199999999999994E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>6.5199999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.5199999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.5199999999999994E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>6.5199999999999994E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -969,10 +1011,10 @@
           </c:marker>
           <c:cat>
             <c:numRef>
-              <c:f>v_n_bottleneck!$C$10:$C$14</c:f>
+              <c:f>v_n_bottleneck!$C$10:$C$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="9"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -987,16 +1029,25 @@
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>96</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>128</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>256</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>512</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>v_n_bottleneck!$E$10:$E$14</c:f>
+              <c:f>v_n_bottleneck!$E$10:$E$17</c:f>
               <c:numCache>
                 <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>6.3E-2</c:v>
                 </c:pt>
@@ -1010,6 +1061,15 @@
                   <c:v>6.3E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
+                  <c:v>6.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.3E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>6.3E-2</c:v>
                 </c:pt>
               </c:numCache>
@@ -2971,10 +3031,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E9D6F212-BBC5-4711-822D-DAEA797CC27E}">
-  <dimension ref="B2:G16"/>
+  <dimension ref="B2:G18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3115,8 +3175,36 @@
       </c>
     </row>
     <row r="16" spans="2:7" x14ac:dyDescent="0.35">
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>128</v>
+      </c>
+      <c r="D16" s="3">
+        <v>6.7900000000000002E-2</v>
+      </c>
+      <c r="E16" s="3">
+        <v>6.2199999999999998E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>256</v>
+      </c>
+      <c r="D17" s="3">
+        <v>3.49E-2</v>
+      </c>
+      <c r="E17" s="3">
+        <v>6.2199999999999998E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3127,10 +3215,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA08A97B-CCCB-472F-8363-00D4C6E11A28}">
-  <dimension ref="B2:E14"/>
+  <dimension ref="B2:E17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -3252,6 +3340,48 @@
         <v>6.3E-2</v>
       </c>
     </row>
+    <row r="15" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B15">
+        <v>5</v>
+      </c>
+      <c r="C15">
+        <v>128</v>
+      </c>
+      <c r="D15" s="3">
+        <v>6.5199999999999994E-2</v>
+      </c>
+      <c r="E15" s="3">
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B16">
+        <v>6</v>
+      </c>
+      <c r="C16">
+        <v>256</v>
+      </c>
+      <c r="D16" s="3">
+        <v>6.5199999999999994E-2</v>
+      </c>
+      <c r="E16" s="3">
+        <v>6.3E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
+      <c r="B17">
+        <v>7</v>
+      </c>
+      <c r="C17">
+        <v>512</v>
+      </c>
+      <c r="D17" s="3">
+        <v>6.5199999999999994E-2</v>
+      </c>
+      <c r="E17" s="3">
+        <v>6.3E-2</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>